<commit_message>
Cálculo feito e melhoria implementada na planilha
</commit_message>
<xml_diff>
--- a/Pontos De Função (FPs).xlsx
+++ b/Pontos De Função (FPs).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos de Função" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Guilherme Bornia</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,6 +38,174 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+O sistema requer salvamento e recuperação confiáveis?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+São necessárias comunicações de dados especializadas?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Há funções de processamento distribuído?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+O sistema rodará em ambiente operacional existente e intensamente utilizado?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+O desempenho é crítico?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+O sistema requer entrada de dados online?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+A entrada de dados online requer múlitplas telas ou operações?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t>Guilherme Bornia:</t>
@@ -50,7 +218,261 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Fonte: http://www.catho.com.br/profissoes/analista-de-sistemas/</t>
+Os Arquivos Lógicos Internos são atualizados online?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+As entradas, saídas e consultas são complexas?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+O processamento interno é complexo?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+O código é projetado para ser reutilizável?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A instalação está incluída no projeto?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+O sistema é projetado para múltiplas instalações em diferentes organizações?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A aplicação é projetada para facilitar a troca e o uso pelo usuário?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Guilherme Bornia</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dividindo o total de FPs pelo número de analistas obtém-se a quantidade de FPs  para cada analista.
+Dividindo a quantidade de FPs  para cada analista pelo esforço máximo que um analista pode realizar por mês obtém-se a quantidade de meses necessários para a realização do projeto.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Meses * Dias Úteis em um Mês * Horas Diárias Trabalhadas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Prazo em Horas / Analistas necessários = Horas de trabalho para cada analista
+Horas de trabalho para cada analista * Salário = Custo total do projeto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Guilherme Bornia:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fonte: http://www.catho.com.br/profissoes/analista-de-sistemas/
+Salário/Mensal = R$ 4.000,00
+Horas Trabalhadas = 160/mês ou 40/semana</t>
         </r>
       </text>
     </comment>
@@ -59,7 +481,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Contagem</t>
   </si>
@@ -179,77 +601,32 @@
     <t>Fatores de Ajuste</t>
   </si>
   <si>
-    <t>Fatores de Ajuste (Fi)</t>
-  </si>
-  <si>
-    <t>ESFORÇO
-( FPs / MÊS )</t>
-  </si>
-  <si>
     <t>FPs</t>
   </si>
   <si>
-    <t>Salário / Mês</t>
-  </si>
-  <si>
-    <t>Funcionários Necessários</t>
-  </si>
-  <si>
-    <t>Analistas de Sist.</t>
-  </si>
-  <si>
-    <t>Melhor Escolha</t>
-  </si>
-  <si>
-    <t>1º</t>
-  </si>
-  <si>
-    <t>2º</t>
-  </si>
-  <si>
-    <t>3º</t>
-  </si>
-  <si>
-    <t>4º</t>
-  </si>
-  <si>
-    <t>5º</t>
-  </si>
-  <si>
-    <t>6º</t>
-  </si>
-  <si>
-    <t>7º</t>
-  </si>
-  <si>
-    <t>8º</t>
-  </si>
-  <si>
-    <t>9º</t>
-  </si>
-  <si>
-    <t>10º</t>
-  </si>
-  <si>
-    <t>11º</t>
-  </si>
-  <si>
-    <t>12º</t>
-  </si>
-  <si>
-    <t>13º</t>
-  </si>
-  <si>
-    <t>14º</t>
-  </si>
-  <si>
-    <t>15º</t>
-  </si>
-  <si>
-    <t>16º</t>
-  </si>
-  <si>
-    <t>17º</t>
+    <t>Fatores de
+Ajuste (Fi)</t>
+  </si>
+  <si>
+    <t>Salário / Hora</t>
+  </si>
+  <si>
+    <t>PRAZO EM
+HORAS</t>
+  </si>
+  <si>
+    <t>ANALISTAS NECESSÁRIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESFORÇO
+( FPs / Mês ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESFORÇO
+( FPs / Hora ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;&lt;&lt;&lt;   Pode ser alterado</t>
   </si>
 </sst>
 </file>
@@ -260,7 +637,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +710,19 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -354,7 +744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -597,47 +987,6 @@
       <left style="medium">
         <color theme="0"/>
       </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="0"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -739,11 +1088,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -785,9 +1186,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -801,13 +1199,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,53 +1223,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -879,26 +1312,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1575,11 +1999,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1601,52 +2025,52 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>1</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>3</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>4</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>6</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <f xml:space="preserve"> Tabela1[[#This Row],[Contagem]] * Tabela1[[#This Row],[Simples]]</f>
         <v>3</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <f xml:space="preserve"> Tabela1[[#This Row],[Contagem]] * Tabela1[[#This Row],[Médio]]</f>
         <v>4</v>
       </c>
@@ -1741,10 +2165,10 @@
         <f xml:space="preserve"> Tabela1[[#This Row],[Contagem]] * Tabela1[[#This Row],[Complexo]]</f>
         <v>0</v>
       </c>
-      <c r="K6" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="32"/>
+      <c r="K6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="38"/>
     </row>
     <row r="7" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
@@ -1774,18 +2198,18 @@
         <f xml:space="preserve"> Tabela1[[#This Row],[Contagem]] * Tabela1[[#This Row],[Complexo]]</f>
         <v>0</v>
       </c>
-      <c r="K7" s="34">
-        <f xml:space="preserve"> G8 * ( 0.65 + ( 0.01 * K11 ) )</f>
-        <v>7.15</v>
-      </c>
-      <c r="L7" s="34"/>
+      <c r="K7" s="40">
+        <f>G8*(0.65+(0.01*K12))</f>
+        <v>10.120000000000001</v>
+      </c>
+      <c r="L7" s="40"/>
     </row>
     <row r="8" spans="2:16" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="3"/>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="14">
         <f>SUM(Tabela1[Resultado
 (Simples)])</f>
@@ -1801,116 +2225,134 @@
 (Complexo)])</f>
         <v>20</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="32"/>
+      <c r="L10" s="38"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="17">
+        <v>3</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>4</v>
+      </c>
+      <c r="G11" s="17">
+        <v>4</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="K12" s="34">
-        <f>SUM(C11:I11,C14:I14)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="34"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="41">
+        <f>SUM(C11:I11,C13:I13)</f>
+        <v>27</v>
+      </c>
+      <c r="L12" s="41"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="17">
+        <v>0</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17">
+        <v>5</v>
+      </c>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17">
+        <v>5</v>
+      </c>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
+      <c r="B14" s="29"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B10:B11"/>
+  <mergeCells count="6">
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="K7:L8"/>
@@ -1919,666 +2361,644 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:J7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="1.7109375" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
+    <col min="2" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="1.7109375" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="2:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
     </row>
-    <row r="3" spans="2:14" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46" t="s">
+    <row r="3" spans="2:16" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="I3" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="44"/>
-      <c r="L3" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="I3" s="56"/>
+      <c r="K3" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="53"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
     </row>
-    <row r="4" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="48">
+    <row r="4" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B4)/$K$8</f>
+        <v>2.024</v>
+      </c>
+      <c r="E4" s="52"/>
+      <c r="F4" s="44">
+        <f>IFERROR(D4*20*8,0)</f>
+        <v>323.84000000000003</v>
+      </c>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46">
+        <f xml:space="preserve"> ( F4 / B4 )  * $K$4</f>
+        <v>8126.8457600000011</v>
+      </c>
+      <c r="I4" s="47"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="59">
+        <f xml:space="preserve"> 4015.24 / 160</f>
+        <v>25.09525</v>
+      </c>
+      <c r="L4" s="59"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="36"/>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="50">
+        <v>2</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B5)/$K$8</f>
+        <v>1.012</v>
+      </c>
+      <c r="E5" s="52"/>
+      <c r="F5" s="44">
+        <f t="shared" ref="F5:F20" si="0">IFERROR(D5*20*8,0)</f>
+        <v>161.92000000000002</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46">
+        <f t="shared" ref="H5:H20" si="1" xml:space="preserve"> ( F5 / B5 )  * $K$4</f>
+        <v>2031.7114400000003</v>
+      </c>
+      <c r="I5" s="47"/>
+      <c r="J5" s="28"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="2:16" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="42">
+        <v>3</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B6)/$K$8</f>
+        <v>0.67466666666666675</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="44">
+        <f t="shared" si="0"/>
+        <v>107.94666666666669</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46">
+        <f t="shared" si="1"/>
+        <v>902.98286222222237</v>
+      </c>
+      <c r="I6" s="47"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="60"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="49"/>
+    </row>
+    <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50">
+        <v>4</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B7)/$K$8</f>
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="44">
+        <f t="shared" si="0"/>
+        <v>80.960000000000008</v>
+      </c>
+      <c r="G7" s="45"/>
+      <c r="H7" s="46">
+        <f t="shared" si="1"/>
+        <v>507.92786000000007</v>
+      </c>
+      <c r="I7" s="47"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="49"/>
+    </row>
+    <row r="8" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42">
         <v>5</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B4,0)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52">
-        <f t="shared" ref="F4:F20" si="0" xml:space="preserve"> D4 * $I$4</f>
-        <v>8800</v>
-      </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="31" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B8)/$K$8</f>
+        <v>0.40479999999999999</v>
+      </c>
+      <c r="E8" s="52"/>
+      <c r="F8" s="44">
+        <f t="shared" si="0"/>
+        <v>64.768000000000001</v>
+      </c>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46">
+        <f t="shared" si="1"/>
+        <v>325.07383040000002</v>
+      </c>
+      <c r="I8" s="47"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="61">
+        <v>5</v>
+      </c>
+      <c r="L8" s="61"/>
+      <c r="M8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="53">
-        <v>4000</v>
-      </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="29">
-        <f xml:space="preserve"> F4 / $I$4</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M4" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="42"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="36">
+    <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="50">
         <v>6</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B5,0)</f>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40">
+      <c r="C9" s="47"/>
+      <c r="D9" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B9)/$K$8</f>
+        <v>0.33733333333333337</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="44">
         <f t="shared" si="0"/>
-        <v>7333.333333333333</v>
-      </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="29">
-        <f xml:space="preserve"> F5 / $I$4</f>
-        <v>1.8333333333333333</v>
-      </c>
-      <c r="M5" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="42"/>
+        <v>53.973333333333343</v>
+      </c>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46">
+        <f t="shared" si="1"/>
+        <v>225.74571555555559</v>
+      </c>
+      <c r="I9" s="47"/>
+      <c r="J9" s="28"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="49"/>
     </row>
-    <row r="6" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36">
+    <row r="10" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="42">
         <v>7</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B6,0)</f>
-        <v>1.5714285714285714</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40">
+      <c r="C10" s="43"/>
+      <c r="D10" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B10)/$K$8</f>
+        <v>0.2891428571428572</v>
+      </c>
+      <c r="E10" s="52"/>
+      <c r="F10" s="44">
         <f t="shared" si="0"/>
-        <v>6285.7142857142853</v>
-      </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="44" t="s">
+        <v>46.26285714285715</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46">
+        <f t="shared" si="1"/>
+        <v>165.85399510204084</v>
+      </c>
+      <c r="I10" s="47"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="29">
-        <f xml:space="preserve"> F6 / $I$4</f>
-        <v>1.5714285714285714</v>
-      </c>
-      <c r="M6" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" s="42"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="49"/>
     </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43">
+    <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="50">
         <v>8</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B7,0)</f>
-        <v>1.375</v>
-      </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40">
+      <c r="C11" s="47"/>
+      <c r="D11" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B11)/$K$8</f>
+        <v>0.253</v>
+      </c>
+      <c r="E11" s="52"/>
+      <c r="F11" s="44">
         <f t="shared" si="0"/>
-        <v>5500</v>
-      </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="29">
-        <f xml:space="preserve"> F7 / $I$4</f>
-        <v>1.375</v>
-      </c>
-      <c r="M7" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="42"/>
+        <v>40.480000000000004</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46">
+        <f t="shared" si="1"/>
+        <v>126.98196500000002</v>
+      </c>
+      <c r="I11" s="47"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="49"/>
     </row>
-    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36">
+    <row r="12" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="42">
         <v>9</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B8,0)</f>
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40">
+      <c r="C12" s="43"/>
+      <c r="D12" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B12)/$K$8</f>
+        <v>0.22488888888888892</v>
+      </c>
+      <c r="E12" s="52"/>
+      <c r="F12" s="44">
         <f t="shared" si="0"/>
-        <v>4888.8888888888896</v>
-      </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="29">
-        <f t="shared" ref="L8:L19" si="1" xml:space="preserve"> F8 / $I$4</f>
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="M8" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N8" s="42"/>
+        <v>35.982222222222227</v>
+      </c>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46">
+        <f t="shared" si="1"/>
+        <v>100.33142913580248</v>
+      </c>
+      <c r="I12" s="47"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="61">
+        <f xml:space="preserve"> ( K8 / 20 ) / 8</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="L12" s="61"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="49"/>
     </row>
-    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="36">
+    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="50">
         <v>10</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B9,0)</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40">
+      <c r="C13" s="47"/>
+      <c r="D13" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B13)/$K$8</f>
+        <v>0.2024</v>
+      </c>
+      <c r="E13" s="52"/>
+      <c r="F13" s="44">
         <f t="shared" si="0"/>
-        <v>4400</v>
-      </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="29">
+        <v>32.384</v>
+      </c>
+      <c r="G13" s="45"/>
+      <c r="H13" s="46">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M9" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N9" s="42"/>
+        <v>81.268457600000005</v>
+      </c>
+      <c r="I13" s="47"/>
+      <c r="J13" s="28"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="49"/>
     </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36">
+    <row r="14" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="42">
         <v>11</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B10,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40">
+      <c r="C14" s="43"/>
+      <c r="D14" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B14)/$K$8</f>
+        <v>0.184</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="44">
         <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="29">
+        <v>29.439999999999998</v>
+      </c>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M10" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="42"/>
+        <v>67.164014545454549</v>
+      </c>
+      <c r="I14" s="47"/>
+      <c r="J14" s="28"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="49"/>
     </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="43">
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="50">
         <v>12</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B11,0)</f>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40">
+      <c r="C15" s="47"/>
+      <c r="D15" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B15)/$K$8</f>
+        <v>0.16866666666666669</v>
+      </c>
+      <c r="E15" s="52"/>
+      <c r="F15" s="44">
         <f t="shared" si="0"/>
-        <v>3666.6666666666665</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="29">
+        <v>26.986666666666672</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="H15" s="46">
         <f t="shared" si="1"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="M11" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N11" s="42"/>
+        <v>56.436428888888898</v>
+      </c>
+      <c r="I15" s="47"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="33"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="49"/>
     </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="36">
+    <row r="16" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="42">
         <v>13</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B12,0)</f>
-        <v>0.84615384615384615</v>
-      </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40">
+      <c r="C16" s="43"/>
+      <c r="D16" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B16)/$K$8</f>
+        <v>0.15569230769230771</v>
+      </c>
+      <c r="E16" s="52"/>
+      <c r="F16" s="44">
         <f t="shared" si="0"/>
-        <v>3384.6153846153848</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" s="29">
+        <v>24.910769230769233</v>
+      </c>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46">
         <f t="shared" si="1"/>
-        <v>0.84615384615384615</v>
-      </c>
-      <c r="M12" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="42"/>
+        <v>48.08784473372782</v>
+      </c>
+      <c r="I16" s="47"/>
+      <c r="J16" s="28"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="49"/>
     </row>
-    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="36">
+    <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="50">
         <v>14</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B13,0)</f>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40">
+      <c r="C17" s="47"/>
+      <c r="D17" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B17)/$K$8</f>
+        <v>0.1445714285714286</v>
+      </c>
+      <c r="E17" s="52"/>
+      <c r="F17" s="44">
         <f t="shared" si="0"/>
-        <v>3142.8571428571427</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="29">
+        <v>23.131428571428575</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46">
         <f t="shared" si="1"/>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="M13" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" s="42"/>
+        <v>41.46349877551021</v>
+      </c>
+      <c r="I17" s="47"/>
+      <c r="J17" s="28"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="49"/>
     </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36">
+    <row r="18" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="42">
         <v>15</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B14,0)</f>
-        <v>0.73333333333333328</v>
-      </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40">
+      <c r="C18" s="43"/>
+      <c r="D18" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B18)/$K$8</f>
+        <v>0.13493333333333335</v>
+      </c>
+      <c r="E18" s="52"/>
+      <c r="F18" s="44">
         <f t="shared" si="0"/>
-        <v>2933.333333333333</v>
-      </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="29">
+        <v>21.589333333333336</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46">
         <f t="shared" si="1"/>
-        <v>0.73333333333333328</v>
-      </c>
-      <c r="M14" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N14" s="42"/>
+        <v>36.119314488888897</v>
+      </c>
+      <c r="I18" s="47"/>
+      <c r="J18" s="28"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="49"/>
     </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="43">
+    <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="50">
         <v>16</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B15,0)</f>
-        <v>0.6875</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40">
+      <c r="C19" s="47"/>
+      <c r="D19" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B19)/$K$8</f>
+        <v>0.1265</v>
+      </c>
+      <c r="E19" s="52"/>
+      <c r="F19" s="44">
         <f t="shared" si="0"/>
-        <v>2750</v>
-      </c>
-      <c r="G15" s="37"/>
-      <c r="H15" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="L15" s="29">
+        <v>20.240000000000002</v>
+      </c>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46">
         <f t="shared" si="1"/>
-        <v>0.6875</v>
-      </c>
-      <c r="M15" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N15" s="42"/>
+        <v>31.745491250000004</v>
+      </c>
+      <c r="I19" s="47"/>
+      <c r="J19" s="28"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="49"/>
     </row>
-    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36">
+    <row r="20" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="42">
         <v>17</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B16,0)</f>
-        <v>0.6470588235294118</v>
-      </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40">
+      <c r="C20" s="43"/>
+      <c r="D20" s="51">
+        <f>('Pontos de Função'!$K$7/'Custo Benefício'!B20)/$K$8</f>
+        <v>0.11905882352941177</v>
+      </c>
+      <c r="E20" s="52"/>
+      <c r="F20" s="44">
         <f t="shared" si="0"/>
-        <v>2588.2352941176473</v>
-      </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="29">
+        <v>19.049411764705884</v>
+      </c>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46">
         <f t="shared" si="1"/>
-        <v>0.6470588235294118</v>
-      </c>
-      <c r="M16" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="42"/>
+        <v>28.120573564013842</v>
+      </c>
+      <c r="I20" s="47"/>
+      <c r="J20" s="28"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="49"/>
     </row>
-    <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="36">
-        <v>18</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B17,0)</f>
-        <v>0.61111111111111116</v>
-      </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40">
-        <f t="shared" si="0"/>
-        <v>2444.4444444444448</v>
-      </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="29">
-        <f t="shared" si="1"/>
-        <v>0.61111111111111116</v>
-      </c>
-      <c r="M17" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="42"/>
-    </row>
-    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36">
-        <v>19</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B18,0)</f>
-        <v>0.57894736842105265</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40">
-        <f t="shared" si="0"/>
-        <v>2315.7894736842104</v>
-      </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="L18" s="29">
-        <f t="shared" si="1"/>
-        <v>0.57894736842105265</v>
-      </c>
-      <c r="M18" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N18" s="42"/>
-    </row>
-    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="43">
-        <v>20</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B19,0)</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40">
-        <f t="shared" si="0"/>
-        <v>2200</v>
-      </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="K19" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="L19" s="29">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M19" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N19" s="42"/>
-    </row>
-    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="36">
-        <v>21</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38">
-        <f>IFERROR( 'Pontos de Função'!$G$8 / B20,0)</f>
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40">
-        <f t="shared" si="0"/>
-        <v>2095.2380952380954</v>
-      </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="29">
-        <f xml:space="preserve"> F20 / $I$4</f>
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="M20" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="N20" s="42"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
+  <mergeCells count="94">
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado o número de FPs/mês
</commit_message>
<xml_diff>
--- a/Pontos De Função (FPs).xlsx
+++ b/Pontos De Função (FPs).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\Graduação\2016\3º Semestre\Engenharia de Software ll - Pedro Ivo Garcia Nunes SI304 B\Atividades\03 - Atividade Prática\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\Graduação\2016\3º Semestre\Engenharia de Software ll - Pedro Ivo Garcia Nunes SI304 B\Atividades\SI304\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1261,40 +1261,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1306,23 +1312,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2373,7 +2373,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:L4"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2390,98 +2390,98 @@
   <sheetData>
     <row r="1" spans="2:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
     </row>
     <row r="3" spans="2:16" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="57" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="55" t="s">
+      <c r="E3" s="62"/>
+      <c r="F3" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="K3" s="53" t="s">
+      <c r="I3" s="58"/>
+      <c r="K3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="53"/>
+      <c r="L3" s="46"/>
       <c r="M3" s="30"/>
       <c r="N3" s="34"/>
       <c r="O3" s="34"/>
       <c r="P3" s="34"/>
     </row>
     <row r="4" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42">
+      <c r="B4" s="59">
         <v>1</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="51">
+      <c r="C4" s="60"/>
+      <c r="D4" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B4)/$K$8</f>
-        <v>2.024</v>
-      </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="44">
+        <v>1.6866666666666668</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="54">
         <f>IFERROR(D4*20*8,0)</f>
-        <v>323.84000000000003</v>
-      </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="46">
+        <v>269.86666666666667</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="50">
         <f xml:space="preserve"> ( F4 / B4 )  * $K$4</f>
-        <v>8126.8457600000011</v>
-      </c>
-      <c r="I4" s="47"/>
+        <v>6772.3714666666665</v>
+      </c>
+      <c r="I4" s="51"/>
       <c r="J4" s="28"/>
-      <c r="K4" s="59">
+      <c r="K4" s="47">
         <f xml:space="preserve"> 4015.24 / 160</f>
         <v>25.09525</v>
       </c>
-      <c r="L4" s="59"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="31"/>
       <c r="N4" s="32"/>
       <c r="O4" s="35"/>
       <c r="P4" s="36"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="50">
+      <c r="B5" s="53">
         <v>2</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="51">
+      <c r="C5" s="51"/>
+      <c r="D5" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B5)/$K$8</f>
-        <v>1.012</v>
-      </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="44">
+        <v>0.84333333333333338</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="54">
         <f t="shared" ref="F5:F20" si="0">IFERROR(D5*20*8,0)</f>
-        <v>161.92000000000002</v>
-      </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46">
+        <v>134.93333333333334</v>
+      </c>
+      <c r="G5" s="55"/>
+      <c r="H5" s="50">
         <f t="shared" ref="H5:H20" si="1" xml:space="preserve"> ( F5 / B5 )  * $K$4</f>
-        <v>2031.7114400000003</v>
-      </c>
-      <c r="I5" s="47"/>
+        <v>1693.0928666666666</v>
+      </c>
+      <c r="I5" s="51"/>
       <c r="J5" s="28"/>
       <c r="M5" s="31"/>
       <c r="N5" s="32"/>
@@ -2489,422 +2489,500 @@
       <c r="P5" s="36"/>
     </row>
     <row r="6" spans="2:16" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42">
+      <c r="B6" s="59">
         <v>3</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="51">
+      <c r="C6" s="60"/>
+      <c r="D6" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B6)/$K$8</f>
-        <v>0.67466666666666675</v>
-      </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="44">
+        <v>0.56222222222222229</v>
+      </c>
+      <c r="E6" s="43"/>
+      <c r="F6" s="54">
         <f t="shared" si="0"/>
-        <v>107.94666666666669</v>
-      </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46">
+        <v>89.955555555555563</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="50">
         <f t="shared" si="1"/>
-        <v>902.98286222222237</v>
-      </c>
-      <c r="I6" s="47"/>
+        <v>752.48571851851852</v>
+      </c>
+      <c r="I6" s="51"/>
       <c r="J6" s="28"/>
-      <c r="K6" s="60" t="s">
+      <c r="K6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="60"/>
+      <c r="L6" s="48"/>
       <c r="M6" s="31"/>
       <c r="N6" s="32"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="49"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="45"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50">
+      <c r="B7" s="53">
         <v>4</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="51">
+      <c r="C7" s="51"/>
+      <c r="D7" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B7)/$K$8</f>
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="44">
+        <v>0.42166666666666669</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="54">
         <f t="shared" si="0"/>
-        <v>80.960000000000008</v>
-      </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="46">
+        <v>67.466666666666669</v>
+      </c>
+      <c r="G7" s="55"/>
+      <c r="H7" s="50">
         <f t="shared" si="1"/>
-        <v>507.92786000000007</v>
-      </c>
-      <c r="I7" s="47"/>
+        <v>423.27321666666666</v>
+      </c>
+      <c r="I7" s="51"/>
       <c r="J7" s="28"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
       <c r="M7" s="31"/>
       <c r="N7" s="32"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="45"/>
     </row>
     <row r="8" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="42">
+      <c r="B8" s="59">
         <v>5</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="51">
+      <c r="C8" s="60"/>
+      <c r="D8" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B8)/$K$8</f>
-        <v>0.40479999999999999</v>
-      </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="44">
+        <v>0.33733333333333332</v>
+      </c>
+      <c r="E8" s="43"/>
+      <c r="F8" s="54">
         <f t="shared" si="0"/>
-        <v>64.768000000000001</v>
-      </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46">
+        <v>53.973333333333329</v>
+      </c>
+      <c r="G8" s="55"/>
+      <c r="H8" s="50">
         <f t="shared" si="1"/>
-        <v>325.07383040000002</v>
-      </c>
-      <c r="I8" s="47"/>
+        <v>270.89485866666666</v>
+      </c>
+      <c r="I8" s="51"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="61">
-        <v>5</v>
-      </c>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62" t="s">
+      <c r="K8" s="49">
+        <v>6</v>
+      </c>
+      <c r="L8" s="49"/>
+      <c r="M8" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="50">
+      <c r="B9" s="53">
         <v>6</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="51">
+      <c r="C9" s="51"/>
+      <c r="D9" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B9)/$K$8</f>
-        <v>0.33733333333333337</v>
-      </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="44">
+        <v>0.28111111111111114</v>
+      </c>
+      <c r="E9" s="43"/>
+      <c r="F9" s="54">
         <f t="shared" si="0"/>
-        <v>53.973333333333343</v>
-      </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="46">
+        <v>44.977777777777781</v>
+      </c>
+      <c r="G9" s="55"/>
+      <c r="H9" s="50">
         <f t="shared" si="1"/>
-        <v>225.74571555555559</v>
-      </c>
-      <c r="I9" s="47"/>
+        <v>188.12142962962963</v>
+      </c>
+      <c r="I9" s="51"/>
       <c r="J9" s="28"/>
       <c r="M9" s="31"/>
       <c r="N9" s="32"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="49"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="45"/>
     </row>
     <row r="10" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="42">
+      <c r="B10" s="59">
         <v>7</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="51">
+      <c r="C10" s="60"/>
+      <c r="D10" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B10)/$K$8</f>
-        <v>0.2891428571428572</v>
-      </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="44">
+        <v>0.240952380952381</v>
+      </c>
+      <c r="E10" s="43"/>
+      <c r="F10" s="54">
         <f t="shared" si="0"/>
-        <v>46.26285714285715</v>
-      </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="46">
+        <v>38.552380952380958</v>
+      </c>
+      <c r="G10" s="55"/>
+      <c r="H10" s="50">
         <f t="shared" si="1"/>
-        <v>165.85399510204084</v>
-      </c>
-      <c r="I10" s="47"/>
+        <v>138.21166258503402</v>
+      </c>
+      <c r="I10" s="51"/>
       <c r="J10" s="28"/>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="60"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="31"/>
       <c r="N10" s="32"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="49"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="45"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="50">
+      <c r="B11" s="53">
         <v>8</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="51">
+      <c r="C11" s="51"/>
+      <c r="D11" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B11)/$K$8</f>
-        <v>0.253</v>
-      </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="44">
+        <v>0.21083333333333334</v>
+      </c>
+      <c r="E11" s="43"/>
+      <c r="F11" s="54">
         <f t="shared" si="0"/>
-        <v>40.480000000000004</v>
-      </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="46">
+        <v>33.733333333333334</v>
+      </c>
+      <c r="G11" s="55"/>
+      <c r="H11" s="50">
         <f t="shared" si="1"/>
-        <v>126.98196500000002</v>
-      </c>
-      <c r="I11" s="47"/>
+        <v>105.81830416666666</v>
+      </c>
+      <c r="I11" s="51"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
       <c r="M11" s="31"/>
       <c r="N11" s="32"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="49"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
     </row>
     <row r="12" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="42">
+      <c r="B12" s="59">
         <v>9</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="51">
+      <c r="C12" s="60"/>
+      <c r="D12" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B12)/$K$8</f>
-        <v>0.22488888888888892</v>
-      </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="44">
+        <v>0.18740740740740744</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="F12" s="54">
         <f t="shared" si="0"/>
-        <v>35.982222222222227</v>
-      </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="46">
+        <v>29.985185185185191</v>
+      </c>
+      <c r="G12" s="55"/>
+      <c r="H12" s="50">
         <f t="shared" si="1"/>
-        <v>100.33142913580248</v>
-      </c>
-      <c r="I12" s="47"/>
+        <v>83.609524279835398</v>
+      </c>
+      <c r="I12" s="51"/>
       <c r="J12" s="28"/>
-      <c r="K12" s="61">
+      <c r="K12" s="49">
         <f xml:space="preserve"> ( K8 / 20 ) / 8</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="L12" s="61"/>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="L12" s="49"/>
       <c r="M12" s="31"/>
       <c r="N12" s="32"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="45"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="50">
+      <c r="B13" s="53">
         <v>10</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="51">
+      <c r="C13" s="51"/>
+      <c r="D13" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B13)/$K$8</f>
-        <v>0.2024</v>
-      </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="44">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="54">
         <f t="shared" si="0"/>
-        <v>32.384</v>
-      </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46">
+        <v>26.986666666666665</v>
+      </c>
+      <c r="G13" s="55"/>
+      <c r="H13" s="50">
         <f t="shared" si="1"/>
-        <v>81.268457600000005</v>
-      </c>
-      <c r="I13" s="47"/>
+        <v>67.723714666666666</v>
+      </c>
+      <c r="I13" s="51"/>
       <c r="J13" s="28"/>
       <c r="M13" s="31"/>
       <c r="N13" s="32"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="49"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42">
+      <c r="B14" s="59">
         <v>11</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="51">
+      <c r="C14" s="60"/>
+      <c r="D14" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B14)/$K$8</f>
-        <v>0.184</v>
-      </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="44">
+        <v>0.15333333333333335</v>
+      </c>
+      <c r="E14" s="43"/>
+      <c r="F14" s="54">
         <f t="shared" si="0"/>
-        <v>29.439999999999998</v>
-      </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46">
+        <v>24.533333333333335</v>
+      </c>
+      <c r="G14" s="55"/>
+      <c r="H14" s="50">
         <f t="shared" si="1"/>
-        <v>67.164014545454549</v>
-      </c>
-      <c r="I14" s="47"/>
+        <v>55.970012121212122</v>
+      </c>
+      <c r="I14" s="51"/>
       <c r="J14" s="28"/>
       <c r="M14" s="31"/>
       <c r="N14" s="32"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="49"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="45"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="50">
+      <c r="B15" s="53">
         <v>12</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="51">
+      <c r="C15" s="51"/>
+      <c r="D15" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B15)/$K$8</f>
-        <v>0.16866666666666669</v>
-      </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="44">
+        <v>0.14055555555555557</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="54">
         <f t="shared" si="0"/>
-        <v>26.986666666666672</v>
-      </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46">
+        <v>22.488888888888891</v>
+      </c>
+      <c r="G15" s="55"/>
+      <c r="H15" s="50">
         <f t="shared" si="1"/>
-        <v>56.436428888888898</v>
-      </c>
-      <c r="I15" s="47"/>
+        <v>47.030357407407408</v>
+      </c>
+      <c r="I15" s="51"/>
       <c r="J15" s="28"/>
       <c r="K15" s="33"/>
       <c r="M15" s="31"/>
       <c r="N15" s="32"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="49"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="45"/>
     </row>
     <row r="16" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42">
+      <c r="B16" s="59">
         <v>13</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="51">
+      <c r="C16" s="60"/>
+      <c r="D16" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B16)/$K$8</f>
-        <v>0.15569230769230771</v>
-      </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="44">
+        <v>0.12974358974358977</v>
+      </c>
+      <c r="E16" s="43"/>
+      <c r="F16" s="54">
         <f t="shared" si="0"/>
-        <v>24.910769230769233</v>
-      </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="46">
+        <v>20.758974358974363</v>
+      </c>
+      <c r="G16" s="55"/>
+      <c r="H16" s="50">
         <f t="shared" si="1"/>
-        <v>48.08784473372782</v>
-      </c>
-      <c r="I16" s="47"/>
+        <v>40.073203944773184</v>
+      </c>
+      <c r="I16" s="51"/>
       <c r="J16" s="28"/>
       <c r="M16" s="31"/>
       <c r="N16" s="32"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="49"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="45"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="50">
+      <c r="B17" s="53">
         <v>14</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="51">
+      <c r="C17" s="51"/>
+      <c r="D17" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B17)/$K$8</f>
-        <v>0.1445714285714286</v>
-      </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="44">
+        <v>0.1204761904761905</v>
+      </c>
+      <c r="E17" s="43"/>
+      <c r="F17" s="54">
         <f t="shared" si="0"/>
-        <v>23.131428571428575</v>
-      </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46">
+        <v>19.276190476190479</v>
+      </c>
+      <c r="G17" s="55"/>
+      <c r="H17" s="50">
         <f t="shared" si="1"/>
-        <v>41.46349877551021</v>
-      </c>
-      <c r="I17" s="47"/>
+        <v>34.552915646258505</v>
+      </c>
+      <c r="I17" s="51"/>
       <c r="J17" s="28"/>
       <c r="M17" s="31"/>
       <c r="N17" s="32"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="49"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="45"/>
     </row>
     <row r="18" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42">
+      <c r="B18" s="59">
         <v>15</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="51">
+      <c r="C18" s="60"/>
+      <c r="D18" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B18)/$K$8</f>
-        <v>0.13493333333333335</v>
-      </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="44">
+        <v>0.11244444444444446</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="F18" s="54">
         <f t="shared" si="0"/>
-        <v>21.589333333333336</v>
-      </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="46">
+        <v>17.991111111111113</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="H18" s="50">
         <f t="shared" si="1"/>
-        <v>36.119314488888897</v>
-      </c>
-      <c r="I18" s="47"/>
+        <v>30.099428740740741</v>
+      </c>
+      <c r="I18" s="51"/>
       <c r="J18" s="28"/>
       <c r="M18" s="31"/>
       <c r="N18" s="32"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="49"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="45"/>
     </row>
     <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="50">
+      <c r="B19" s="53">
         <v>16</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="51">
+      <c r="C19" s="51"/>
+      <c r="D19" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B19)/$K$8</f>
-        <v>0.1265</v>
-      </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="44">
+        <v>0.10541666666666667</v>
+      </c>
+      <c r="E19" s="43"/>
+      <c r="F19" s="54">
         <f t="shared" si="0"/>
-        <v>20.240000000000002</v>
-      </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46">
+        <v>16.866666666666667</v>
+      </c>
+      <c r="G19" s="55"/>
+      <c r="H19" s="50">
         <f t="shared" si="1"/>
-        <v>31.745491250000004</v>
-      </c>
-      <c r="I19" s="47"/>
+        <v>26.454576041666666</v>
+      </c>
+      <c r="I19" s="51"/>
       <c r="J19" s="28"/>
       <c r="M19" s="31"/>
       <c r="N19" s="32"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="49"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="42">
+      <c r="B20" s="59">
         <v>17</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="51">
+      <c r="C20" s="60"/>
+      <c r="D20" s="42">
         <f>('Pontos de Função'!$K$7/'Custo Benefício'!B20)/$K$8</f>
-        <v>0.11905882352941177</v>
-      </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="44">
+        <v>9.9215686274509815E-2</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="F20" s="54">
         <f t="shared" si="0"/>
-        <v>19.049411764705884</v>
-      </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46">
+        <v>15.874509803921571</v>
+      </c>
+      <c r="G20" s="55"/>
+      <c r="H20" s="50">
         <f t="shared" si="1"/>
-        <v>28.120573564013842</v>
-      </c>
-      <c r="I20" s="47"/>
+        <v>23.433811303344871</v>
+      </c>
+      <c r="I20" s="51"/>
       <c r="J20" s="28"/>
       <c r="M20" s="31"/>
       <c r="N20" s="32"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="49"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="45"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
@@ -2921,84 +2999,6 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>